<commit_message>
added raspberry to elektrik; wellrohre
</commit_message>
<xml_diff>
--- a/Elektrik/12V/12VAuslegung.xlsx
+++ b/Elektrik/12V/12VAuslegung.xlsx
@@ -522,9 +522,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>185760</xdr:colOff>
+      <xdr:colOff>185400</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -538,12 +538,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15733800" y="5531400"/>
-          <a:ext cx="6827400" cy="3807360"/>
+          <a:ext cx="6827040" cy="3807000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -559,9 +559,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>335520</xdr:colOff>
+      <xdr:colOff>335160</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -575,12 +575,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17018640" y="2623320"/>
-          <a:ext cx="4361400" cy="2447280"/>
+          <a:ext cx="4361040" cy="2446920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -596,9 +596,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>480240</xdr:colOff>
+      <xdr:colOff>479880</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>55080</xdr:rowOff>
+      <xdr:rowOff>54720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -612,12 +612,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9491040" y="4035240"/>
-          <a:ext cx="4474440" cy="2980440"/>
+          <a:ext cx="4474080" cy="2980080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -634,8 +634,8 @@
   </sheetPr>
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="N12" s="0" t="n">
         <f aca="false">2*(G10+G11+G12+G13+G13+G14+G9+G17+G15+G16)</f>
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,22 +1134,22 @@
         <v>12</v>
       </c>
       <c r="D15" s="4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E15" s="4" t="n">
         <f aca="false">D15/C15</f>
-        <v>0.416666666666667</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="F15" s="4" t="n">
         <f aca="false">B15*E15</f>
-        <v>0.416666666666667</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="G15" s="4" t="n">
         <v>4</v>
       </c>
       <c r="H15" s="4" t="n">
         <f aca="false">(G15*2*F15)/(C15*$N$4*$N$6)</f>
-        <v>0.242897672068711</v>
+        <v>0.485795344137422</v>
       </c>
       <c r="I15" s="4" t="n">
         <v>1.5</v>
@@ -1163,7 +1163,7 @@
         <v>33</v>
       </c>
       <c r="B16" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>12</v>
@@ -1177,14 +1177,14 @@
       </c>
       <c r="F16" s="4" t="n">
         <f aca="false">B16*E16</f>
-        <v>0</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="G16" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H16" s="4" t="n">
         <f aca="false">(G16*2*F16)/(C16*$N$4*$N$6)</f>
-        <v>0</v>
+        <v>0.242897672068711</v>
       </c>
       <c r="I16" s="4" t="n">
         <v>1.5</v>
@@ -1205,14 +1205,14 @@
       </c>
       <c r="F17" s="4" t="n">
         <f aca="false">SUM(F9:F16)</f>
-        <v>5.6</v>
+        <v>6.43333333333333</v>
       </c>
       <c r="G17" s="4" t="n">
         <v>0.5</v>
       </c>
       <c r="H17" s="4" t="n">
         <f aca="false">(G17*2*F17)/(C17*$N$4*$N$6)</f>
-        <v>0.408068089075434</v>
+        <v>0.468792507092612</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,7 +1497,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>